<commit_message>
excel files for dirac performance
</commit_message>
<xml_diff>
--- a/test/Performance Data/MGPU/Benchmark_Excel/gtx560Ti/Bulk Insert/gtx560Ti_benchmarkBulkInsert_aleacubase_vs_moderngpu_Float32.xlsx
+++ b/test/Performance Data/MGPU/Benchmark_Excel/gtx560Ti/Bulk Insert/gtx560Ti_benchmarkBulkInsert_aleacubase_vs_moderngpu_Float32.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\dev\GitHub\Alea.cuExtension\test\Test.Alea.CUDA.Extension.MGPU\Performance Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\dev\GitHub\Alea.cuExtension\test\Performance Data\MGPU\Benchmark_Excel\gtx560Ti\Bulk Insert\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -361,11 +361,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2034868880"/>
-        <c:axId val="2034872688"/>
+        <c:axId val="-2081296096"/>
+        <c:axId val="-2081295552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2034868880"/>
+        <c:axId val="-2081296096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -375,12 +375,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2034872688"/>
+        <c:crossAx val="-2081295552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2034872688"/>
+        <c:axId val="-2081295552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -391,7 +391,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2034868880"/>
+        <c:crossAx val="-2081296096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -648,11 +648,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2030363376"/>
-        <c:axId val="2034869968"/>
+        <c:axId val="-2081843104"/>
+        <c:axId val="-2081840928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2030363376"/>
+        <c:axId val="-2081843104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -662,12 +662,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2034869968"/>
+        <c:crossAx val="-2081840928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2034869968"/>
+        <c:axId val="-2081840928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -678,7 +678,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2030363376"/>
+        <c:crossAx val="-2081843104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>

</xml_diff>

<commit_message>
nsight timing output for f#
</commit_message>
<xml_diff>
--- a/test/Performance Data/MGPU/Benchmark_Excel/gtx560Ti/Bulk Insert/gtx560Ti_benchmarkBulkInsert_aleacubase_vs_moderngpu_Float32.xlsx
+++ b/test/Performance Data/MGPU/Benchmark_Excel/gtx560Ti/Bulk Insert/gtx560Ti_benchmarkBulkInsert_aleacubase_vs_moderngpu_Float32.xlsx
@@ -133,21 +133,37 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="120"/>
+      <c14:style val="104"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="20"/>
+      <c:style val="4"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
@@ -158,6 +174,39 @@
       </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -179,6 +228,73 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:shade val="76000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:shade val="76000"/>
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:shade val="76000"/>
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:shade val="76000"/>
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:shade val="76000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$6:$B$15</c:f>
@@ -273,6 +389,73 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:tint val="77000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:tint val="77000"/>
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:tint val="77000"/>
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:tint val="77000"/>
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:tint val="77000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$6:$B$15</c:f>
@@ -361,50 +544,206 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2081296096"/>
-        <c:axId val="-2081295552"/>
+        <c:axId val="1278266688"/>
+        <c:axId val="1278259072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2081296096"/>
+        <c:axId val="1278266688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2081295552"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1278259072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2081295552"/>
+        <c:axId val="1278259072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2081296096"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1278266688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -430,11 +769,27 @@
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
@@ -445,6 +800,39 @@
       </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -466,6 +854,73 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:shade val="76000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:shade val="76000"/>
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5">
+                      <a:shade val="76000"/>
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:shade val="76000"/>
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:shade val="76000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$19:$B$28</c:f>
@@ -560,6 +1015,73 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:tint val="77000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:tint val="77000"/>
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5">
+                      <a:tint val="77000"/>
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:tint val="77000"/>
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:tint val="77000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$19:$B$28</c:f>
@@ -648,56 +1170,1228 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2081843104"/>
-        <c:axId val="-2081840928"/>
+        <c:axId val="1098970128"/>
+        <c:axId val="1098970672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2081843104"/>
+        <c:axId val="1098970128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2081840928"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1098970672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2081840928"/>
+        <c:axId val="1098970672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2081843104"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1098970128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="15">
+  <a:schemeClr val="accent2"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="18">
+  <a:schemeClr val="accent5"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1030,7 +2724,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45:B54"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1404,7 +3100,7 @@
         <v>10000</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>5.556</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -1418,7 +3114,7 @@
         <v>50000</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>10.042999999999999</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -1432,7 +3128,7 @@
         <v>100000</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>17.686</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -1446,7 +3142,7 @@
         <v>200000</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>31.712</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -1460,7 +3156,7 @@
         <v>500000</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>75.599999999999994</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1474,7 +3170,7 @@
         <v>1000000</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>147.68899999999999</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1488,7 +3184,7 @@
         <v>2000000</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>292.178</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1502,7 +3198,7 @@
         <v>5000000</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>724.93299999999999</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1516,7 +3212,7 @@
         <v>10000000</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>1446.876</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1530,7 +3226,7 @@
         <v>20000000</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>2888.74</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1563,7 +3259,7 @@
         <v>10000</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>9.5749999999999993</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -1577,7 +3273,7 @@
         <v>50000</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>25.300999999999998</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -1591,7 +3287,7 @@
         <v>100000</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>29.033999999999999</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -1605,7 +3301,7 @@
         <v>200000</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>31.704000000000001</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -1619,7 +3315,7 @@
         <v>500000</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>34.904000000000003</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -1633,7 +3329,7 @@
         <v>1000000</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>47.843000000000004</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -1647,7 +3343,7 @@
         <v>2000000</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>94.322000000000003</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -1661,7 +3357,7 @@
         <v>5000000</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>255.27199999999999</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -1675,7 +3371,7 @@
         <v>10000000</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>529.06600000000003</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -1689,7 +3385,7 @@
         <v>20000000</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>1111.923</v>
       </c>
       <c r="C54">
         <v>0</v>

</xml_diff>